<commit_message>
Updated ITA model - 2025-07-31 19:07
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/scen_tsparameters_ts_108.xlsx
+++ b/VerveStacks_ITA/SuppXLS/scen_tsparameters_ts_108.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CAD5FD-DCC5-420B-9A09-DC58C3675FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E8448F-3BA8-4C09-A058-F721DB0076ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -921,10 +921,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h10,Tc0917h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h11,Wb0121h09,Tc0917h08,Tc0917h17,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Wb0121h13,RaD,Wb0122h11,Wb0122h15,TaD,Wb0122h12,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0916h12,Tc0917h18,Wb0121h08,Wb0121h18,Wb0121h14,Wb0121h16</t>
-  </si>
-  <si>
-    <t>Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,SaP,Tc0916h06,Tc0917h01,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0916h04,TaP,Tc0916h21,Wb0121h20,Wb0122h04,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,RaN,Tc0917h20,Wb0122h20,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,TaN,Tc0916h03,Tc0916h23,Tc0917h24,Wb0121h05,Wb0121h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22</t>
+    <t>Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,RaD,Wb0122h11,Wb0122h15,Tc0917h08,Tc0917h17,Tc0916h11,Wb0121h09,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h13,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Wb0121h14,Wb0121h16,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h10,Tc0917h14,Tc0917h11,WaD,Wb0122h08,Wb0122h18,TaD,Wb0122h12,Tc0916h12</t>
+  </si>
+  <si>
+    <t>Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h04,SaP,Tc0916h06,Tc0917h01,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,TaN,Tc0916h03,Tc0916h23,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Wb0121h05,Wb0121h24,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0916h24,Tc0917h05,Tc0917h19,RaN,Tc0917h20,Wb0122h20,Tc0917h24</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,SaP,Tc0916h06,Tc0917h01,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0916h04,TaP,Tc0916h21,Wb0121h20,Wb0122h04,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,RaN,Tc0917h20,Wb0122h20,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,TaN,Tc0916h03,Tc0916h23,Tc0917h24,Wb0121h05,Wb0121h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22</v>
+        <v>Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h04,SaP,Tc0916h06,Tc0917h01,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,TaN,Tc0916h03,Tc0916h23,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Wb0121h05,Wb0121h24,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0916h24,Tc0917h05,Tc0917h19,RaN,Tc0917h20,Wb0122h20,Tc0917h24</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h10,Tc0917h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h11,Wb0121h09,Tc0917h08,Tc0917h17,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Wb0121h13,RaD,Wb0122h11,Wb0122h15,TaD,Wb0122h12,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0916h12,Tc0917h18,Wb0121h08,Wb0121h18,Wb0121h14,Wb0121h16</v>
+        <v>Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,RaD,Wb0122h11,Wb0122h15,Tc0917h08,Tc0917h17,Tc0916h11,Wb0121h09,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h13,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Wb0121h14,Wb0121h16,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h10,Tc0917h14,Tc0917h11,WaD,Wb0122h08,Wb0122h18,TaD,Wb0122h12,Tc0916h12</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2140,7 +2140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02C6277-5B25-441C-B3EF-E33BAEBFC0A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B839D9C8-D2AA-4F1C-A7F6-36C8C506FF6A}">
   <dimension ref="B2:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2997,7 +2997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28A4006-2FB8-4BED-B91A-45A2830FD510}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4B145B-84EF-4AAD-BFF1-CCDCF5981BFB}">
   <dimension ref="B2:O111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3076,10 +3076,10 @@
         <v>180</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="N4">
-        <v>0.40439611291068944</v>
+        <v>0.22555529847292916</v>
       </c>
       <c r="O4" t="s">
         <v>300</v>
@@ -3111,10 +3111,10 @@
         <v>180</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="N5">
-        <v>0.30301943544655247</v>
+        <v>0.26702915316982878</v>
       </c>
       <c r="O5" t="s">
         <v>300</v>
@@ -3146,10 +3146,10 @@
         <v>180</v>
       </c>
       <c r="M6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="N6">
-        <v>0.26702915316982873</v>
+        <v>0.30301943544655252</v>
       </c>
       <c r="O6" t="s">
         <v>300</v>
@@ -3181,10 +3181,10 @@
         <v>180</v>
       </c>
       <c r="M7" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="N7">
-        <v>0.22555529847292913</v>
+        <v>0.40439611291068944</v>
       </c>
       <c r="O7" t="s">
         <v>300</v>
@@ -5900,7 +5900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E5660D-D1C3-4067-8C5C-5B1296D3BAD8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCF04D2-3847-45CF-98AF-6F5600E26BCE}">
   <dimension ref="B2:O211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-31 19:11
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/scen_tsparameters_ts_108.xlsx
+++ b/VerveStacks_ITA/SuppXLS/scen_tsparameters_ts_108.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E8448F-3BA8-4C09-A058-F721DB0076ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E1007C-58FA-4C5E-B475-8071AC0E67A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -921,10 +921,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,RaD,Wb0122h11,Wb0122h15,Tc0917h08,Tc0917h17,Tc0916h11,Wb0121h09,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h13,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Wb0121h14,Wb0121h16,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h10,Tc0917h14,Tc0917h11,WaD,Wb0122h08,Wb0122h18,TaD,Wb0122h12,Tc0916h12</t>
-  </si>
-  <si>
-    <t>Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h04,SaP,Tc0916h06,Tc0917h01,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,TaN,Tc0916h03,Tc0916h23,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Wb0121h05,Wb0121h24,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0916h24,Tc0917h05,Tc0917h19,RaN,Tc0917h20,Wb0122h20,Tc0917h24</t>
+    <t>Tc0917h08,Tc0917h17,Wb0121h14,Wb0121h16,Tc0916h11,Wb0121h09,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,TaD,Wb0122h12,Wb0121h13,RaD,Wb0122h11,Wb0122h15,Tc0916h10,Tc0917h14,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14</t>
+  </si>
+  <si>
+    <t>SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h02,Tc0917h06,WaP,Wb0122h22,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Wb0121h05,Wb0121h24,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,RaN,Tc0917h20,Wb0122h20,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,TaN,Tc0916h03,Tc0916h23,SaP,Tc0916h06,Tc0917h01,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h24,Tc0916h04</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h04,SaP,Tc0916h06,Tc0917h01,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,TaN,Tc0916h03,Tc0916h23,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Wb0121h05,Wb0121h24,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0916h24,Tc0917h05,Tc0917h19,RaN,Tc0917h20,Wb0122h20,Tc0917h24</v>
+        <v>SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h02,Tc0917h06,WaP,Wb0122h22,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Wb0121h05,Wb0121h24,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,RaN,Tc0917h20,Wb0122h20,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,TaN,Tc0916h03,Tc0916h23,SaP,Tc0916h06,Tc0917h01,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h24,Tc0916h04</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,RaD,Wb0122h11,Wb0122h15,Tc0917h08,Tc0917h17,Tc0916h11,Wb0121h09,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h13,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Wb0121h14,Wb0121h16,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h10,Tc0917h14,Tc0917h11,WaD,Wb0122h08,Wb0122h18,TaD,Wb0122h12,Tc0916h12</v>
+        <v>Tc0917h08,Tc0917h17,Wb0121h14,Wb0121h16,Tc0916h11,Wb0121h09,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,TaD,Wb0122h12,Wb0121h13,RaD,Wb0122h11,Wb0122h15,Tc0916h10,Tc0917h14,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2140,7 +2140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B839D9C8-D2AA-4F1C-A7F6-36C8C506FF6A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC30070-D60F-4D96-972C-702F9D8A9181}">
   <dimension ref="B2:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2997,7 +2997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4B145B-84EF-4AAD-BFF1-CCDCF5981BFB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555A3A1A-2417-4539-B9CF-3FD94FCEB49E}">
   <dimension ref="B2:O111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3111,10 +3111,10 @@
         <v>180</v>
       </c>
       <c r="M5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="N5">
-        <v>0.26702915316982878</v>
+        <v>0.30301943544655252</v>
       </c>
       <c r="O5" t="s">
         <v>300</v>
@@ -3146,10 +3146,10 @@
         <v>180</v>
       </c>
       <c r="M6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N6">
-        <v>0.30301943544655252</v>
+        <v>0.4043961129106895</v>
       </c>
       <c r="O6" t="s">
         <v>300</v>
@@ -3181,10 +3181,10 @@
         <v>180</v>
       </c>
       <c r="M7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="N7">
-        <v>0.40439611291068944</v>
+        <v>0.26702915316982878</v>
       </c>
       <c r="O7" t="s">
         <v>300</v>
@@ -5900,7 +5900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCF04D2-3847-45CF-98AF-6F5600E26BCE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A861F9F5-CB4A-4F82-88A3-4147C1230752}">
   <dimension ref="B2:O211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-01 02:33
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/scen_tsparameters_ts_108.xlsx
+++ b/VerveStacks_ITA/SuppXLS/scen_tsparameters_ts_108.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E1007C-58FA-4C5E-B475-8071AC0E67A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565E8ED3-198A-41D3-BD2A-567C83A064A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1909" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1933" uniqueCount="302">
   <si>
     <t>UC_N</t>
   </si>
@@ -921,10 +921,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>Tc0917h08,Tc0917h17,Wb0121h14,Wb0121h16,Tc0916h11,Wb0121h09,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,TaD,Wb0122h12,Wb0121h13,RaD,Wb0122h11,Wb0122h15,Tc0916h10,Tc0917h14,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14</t>
-  </si>
-  <si>
-    <t>SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h02,Tc0917h06,WaP,Wb0122h22,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Wb0121h05,Wb0121h24,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,RaN,Tc0917h20,Wb0122h20,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,TaN,Tc0916h03,Tc0916h23,SaP,Tc0916h06,Tc0917h01,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h24,Tc0916h04</t>
+    <t>Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h18,Wb0121h08,Wb0121h18,Wb0121h14,Wb0121h16,Tc0916h11,Wb0121h09,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,TaD,Wb0122h12,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0917h08,Tc0917h17,Tc0916h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Wb0121h13,Tc0917h11,WaD,Wb0122h08,Wb0122h18,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h10,Tc0917h14,RaD,Wb0122h11,Wb0122h15</t>
+  </si>
+  <si>
+    <t>Tc0917h23,Wb0121h02,Wb0121h06,Wb0121h05,Wb0121h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22,TaP,Tc0916h21,Wb0121h20,Wb0122h04,TaN,Tc0916h03,Tc0916h23,RaN,Tc0917h20,Wb0122h20,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h24,Tc0916h04,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0916h24,Tc0917h05,Tc0917h19,SaP,Tc0916h06,Tc0917h01,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h02,Tc0917h06,WaP,Wb0122h22,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Wb0121h05,Wb0121h24,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,RaN,Tc0917h20,Wb0122h20,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,TaN,Tc0916h03,Tc0916h23,SaP,Tc0916h06,Tc0917h01,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h24,Tc0916h04</v>
+        <v>Tc0917h23,Wb0121h02,Wb0121h06,Wb0121h05,Wb0121h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22,TaP,Tc0916h21,Wb0121h20,Wb0122h04,TaN,Tc0916h03,Tc0916h23,RaN,Tc0917h20,Wb0122h20,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h24,Tc0916h04,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0916h24,Tc0917h05,Tc0917h19,SaP,Tc0916h06,Tc0917h01,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>Tc0917h08,Tc0917h17,Wb0121h14,Wb0121h16,Tc0916h11,Wb0121h09,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,TaD,Wb0122h12,Wb0121h13,RaD,Wb0122h11,Wb0122h15,Tc0916h10,Tc0917h14,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14</v>
+        <v>Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h18,Wb0121h08,Wb0121h18,Wb0121h14,Wb0121h16,Tc0916h11,Wb0121h09,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,TaD,Wb0122h12,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0917h08,Tc0917h17,Tc0916h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Wb0121h13,Tc0917h11,WaD,Wb0122h08,Wb0122h18,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h10,Tc0917h14,RaD,Wb0122h11,Wb0122h15</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2140,7 +2140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC30070-D60F-4D96-972C-702F9D8A9181}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB98518D-C10E-4129-8251-208007D084DB}">
   <dimension ref="B2:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2997,7 +2997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555A3A1A-2417-4539-B9CF-3FD94FCEB49E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A79E14D0-70C9-464F-8D10-8B604B7068D6}">
   <dimension ref="B2:O111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3076,10 +3076,10 @@
         <v>180</v>
       </c>
       <c r="M4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="N4">
-        <v>0.22555529847292916</v>
+        <v>0.4043961129106895</v>
       </c>
       <c r="O4" t="s">
         <v>300</v>
@@ -3146,10 +3146,10 @@
         <v>180</v>
       </c>
       <c r="M6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="N6">
-        <v>0.4043961129106895</v>
+        <v>0.22555529847292916</v>
       </c>
       <c r="O6" t="s">
         <v>300</v>
@@ -5900,8 +5900,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A861F9F5-CB4A-4F82-88A3-4147C1230752}">
-  <dimension ref="B2:O211"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB3EB63-0B5C-4A9C-8566-2C04F7653C37}">
+  <dimension ref="B2:O219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5970,7 +5970,7 @@
         <v>178</v>
       </c>
       <c r="J4">
-        <v>0.15044536501940817</v>
+        <v>0.14289521420272036</v>
       </c>
       <c r="M4" t="s">
         <v>14</v>
@@ -5979,7 +5979,7 @@
         <v>178</v>
       </c>
       <c r="O4">
-        <v>0.19271496958451517</v>
+        <v>0.20727306013359903</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.45">
@@ -6002,7 +6002,7 @@
         <v>181</v>
       </c>
       <c r="J5">
-        <v>7.1194979199334679E-2</v>
+        <v>7.9049918900133812E-2</v>
       </c>
       <c r="M5" t="s">
         <v>14</v>
@@ -6011,7 +6011,7 @@
         <v>181</v>
       </c>
       <c r="O5">
-        <v>0.26417119022433222</v>
+        <v>0.30589719182854669</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.45">
@@ -6034,7 +6034,7 @@
         <v>182</v>
       </c>
       <c r="J6">
-        <v>2.3208457890371847E-2</v>
+        <v>2.2965170016217531E-2</v>
       </c>
       <c r="M6" t="s">
         <v>14</v>
@@ -6043,7 +6043,7 @@
         <v>182</v>
       </c>
       <c r="O6">
-        <v>0.16031013287558293</v>
+        <v>0.16806580808227189</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.45">
@@ -6066,7 +6066,7 @@
         <v>183</v>
       </c>
       <c r="J7">
-        <v>0.15021309208390921</v>
+        <v>0.14261699500259242</v>
       </c>
       <c r="M7" t="s">
         <v>14</v>
@@ -6075,7 +6075,7 @@
         <v>183</v>
       </c>
       <c r="O7">
-        <v>0.14569359921939662</v>
+        <v>0.16277845818823344</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.45">
@@ -6098,7 +6098,7 @@
         <v>184</v>
       </c>
       <c r="J8">
-        <v>7.2393301245858327E-2</v>
+        <v>8.0626852872577676E-2</v>
       </c>
       <c r="M8" t="s">
         <v>14</v>
@@ -6107,7 +6107,7 @@
         <v>184</v>
       </c>
       <c r="O8">
-        <v>0.35857132106941414</v>
+        <v>0.33419706528757365</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.45">
@@ -6130,7 +6130,7 @@
         <v>185</v>
       </c>
       <c r="J9">
-        <v>2.2907362766299597E-2</v>
+        <v>2.2465149002500608E-2</v>
       </c>
       <c r="M9" t="s">
         <v>14</v>
@@ -6139,7 +6139,7 @@
         <v>185</v>
       </c>
       <c r="O9">
-        <v>0.11021499745991603</v>
+        <v>0.10300803738580866</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.45">
@@ -6162,7 +6162,7 @@
         <v>186</v>
       </c>
       <c r="J10">
-        <v>0.14189725050443627</v>
+        <v>0.13467968388603346</v>
       </c>
       <c r="M10" t="s">
         <v>14</v>
@@ -6171,7 +6171,7 @@
         <v>186</v>
       </c>
       <c r="O10">
-        <v>0.19591000939477476</v>
+        <v>0.21160461110167583</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.45">
@@ -6194,7 +6194,7 @@
         <v>187</v>
       </c>
       <c r="J11">
-        <v>6.8519745195395179E-2</v>
+        <v>7.6362076728101205E-2</v>
       </c>
       <c r="M11" t="s">
         <v>14</v>
@@ -6203,7 +6203,7 @@
         <v>187</v>
       </c>
       <c r="O11">
-        <v>0.27555959280516396</v>
+        <v>0.31292089659625733</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.45">
@@ -6226,7 +6226,7 @@
         <v>188</v>
       </c>
       <c r="J12">
-        <v>2.210465813063615E-2</v>
+        <v>2.1673698423533425E-2</v>
       </c>
       <c r="M12" t="s">
         <v>14</v>
@@ -6235,7 +6235,7 @@
         <v>188</v>
       </c>
       <c r="O12">
-        <v>0.13392253542789412</v>
+        <v>0.17073368344398987</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.45">
@@ -6258,7 +6258,7 @@
         <v>189</v>
       </c>
       <c r="J13">
-        <v>8.6515258995131786E-5</v>
+        <v>8.5277978427699175E-5</v>
       </c>
       <c r="M13" t="s">
         <v>14</v>
@@ -6290,7 +6290,7 @@
         <v>190</v>
       </c>
       <c r="J14">
-        <v>8.6515258995131786E-5</v>
+        <v>8.3659722628261828E-5</v>
       </c>
       <c r="M14" t="s">
         <v>14</v>
@@ -6322,7 +6322,7 @@
         <v>191</v>
       </c>
       <c r="J15">
-        <v>8.6903540043735579E-5</v>
+        <v>8.3659722628261828E-5</v>
       </c>
       <c r="M15" t="s">
         <v>14</v>
@@ -6354,7 +6354,7 @@
         <v>192</v>
       </c>
       <c r="J16">
-        <v>9.2288998187870096E-5</v>
+        <v>8.4035188010961906E-5</v>
       </c>
       <c r="M16" t="s">
         <v>14</v>
@@ -6386,7 +6386,7 @@
         <v>193</v>
       </c>
       <c r="J17">
-        <v>1.0194554786664627E-4</v>
+        <v>8.9242892869011972E-5</v>
       </c>
       <c r="M17" t="s">
         <v>14</v>
@@ -6418,7 +6418,7 @@
         <v>194</v>
       </c>
       <c r="J18">
-        <v>1.1266987042908287E-4</v>
+        <v>9.8580716936762881E-5</v>
       </c>
       <c r="M18" t="s">
         <v>14</v>
@@ -6450,7 +6450,7 @@
         <v>195</v>
       </c>
       <c r="J19">
-        <v>1.2269140429354661E-4</v>
+        <v>1.0895107080693901E-4</v>
       </c>
       <c r="M19" t="s">
         <v>14</v>
@@ -6482,7 +6482,7 @@
         <v>196</v>
       </c>
       <c r="J20">
-        <v>1.2840690132899434E-4</v>
+        <v>1.1864183233442802E-4</v>
       </c>
       <c r="M20" t="s">
         <v>14</v>
@@ -6514,7 +6514,7 @@
         <v>197</v>
       </c>
       <c r="J21">
-        <v>1.2872529178884946E-4</v>
+        <v>1.2416868276777317E-4</v>
       </c>
       <c r="M21" t="s">
         <v>14</v>
@@ -6546,7 +6546,7 @@
         <v>198</v>
       </c>
       <c r="J22">
-        <v>1.2886507296634681E-4</v>
+        <v>1.2447656438158722E-4</v>
       </c>
       <c r="M22" t="s">
         <v>14</v>
@@ -6578,7 +6578,7 @@
         <v>199</v>
       </c>
       <c r="J23">
-        <v>1.2888448701877701E-4</v>
+        <v>1.2461173191935924E-4</v>
       </c>
       <c r="M23" t="s">
         <v>14</v>
@@ -6610,7 +6610,7 @@
         <v>200</v>
       </c>
       <c r="J24">
-        <v>1.2899320571238605E-4</v>
+        <v>1.2463050518849426E-4</v>
       </c>
       <c r="M24" t="s">
         <v>14</v>
@@ -6642,7 +6642,7 @@
         <v>201</v>
       </c>
       <c r="J25">
-        <v>1.2868646368398908E-4</v>
+        <v>1.2473563549565028E-4</v>
       </c>
       <c r="M25" t="s">
         <v>14</v>
@@ -6674,7 +6674,7 @@
         <v>202</v>
       </c>
       <c r="J26">
-        <v>1.284340810023966E-4</v>
+        <v>1.2443901784331719E-4</v>
       </c>
       <c r="M26" t="s">
         <v>14</v>
@@ -6706,7 +6706,7 @@
         <v>203</v>
       </c>
       <c r="J27">
-        <v>1.2837583884510605E-4</v>
+        <v>1.2419496534456218E-4</v>
       </c>
       <c r="M27" t="s">
         <v>14</v>
@@ -6738,7 +6738,7 @@
         <v>204</v>
       </c>
       <c r="J28">
-        <v>1.2880294799857021E-4</v>
+        <v>1.2413864553715713E-4</v>
       </c>
       <c r="M28" t="s">
         <v>14</v>
@@ -6770,7 +6770,7 @@
         <v>205</v>
       </c>
       <c r="J29">
-        <v>1.2848067472822906E-4</v>
+        <v>1.2455165745812723E-4</v>
       </c>
       <c r="M29" t="s">
         <v>14</v>
@@ -6802,7 +6802,7 @@
         <v>206</v>
       </c>
       <c r="J30">
-        <v>1.2892331512363739E-4</v>
+        <v>1.2424002119048615E-4</v>
       </c>
       <c r="M30" t="s">
         <v>14</v>
@@ -6834,7 +6834,7 @@
         <v>207</v>
       </c>
       <c r="J31">
-        <v>1.277973000826864E-4</v>
+        <v>1.2466805172676426E-4</v>
       </c>
       <c r="M31" t="s">
         <v>14</v>
@@ -6866,7 +6866,7 @@
         <v>208</v>
       </c>
       <c r="J32">
-        <v>1.2460562986316327E-4</v>
+        <v>1.2357920211693405E-4</v>
       </c>
       <c r="M32" t="s">
         <v>14</v>
@@ -6898,7 +6898,7 @@
         <v>209</v>
       </c>
       <c r="J33">
-        <v>1.1843972681133512E-4</v>
+        <v>1.2049287667113939E-4</v>
       </c>
       <c r="M33" t="s">
         <v>14</v>
@@ -6930,7 +6930,7 @@
         <v>210</v>
       </c>
       <c r="J34">
-        <v>1.0097872805562285E-4</v>
+        <v>1.1453048639386216E-4</v>
       </c>
       <c r="M34" t="s">
         <v>14</v>
@@ -6962,7 +6962,7 @@
         <v>211</v>
       </c>
       <c r="J35">
-        <v>9.3609153753122977E-5</v>
+        <v>9.7645808133839704E-5</v>
       </c>
       <c r="M35" t="s">
         <v>14</v>
@@ -6991,16 +6991,16 @@
         <v>295</v>
       </c>
       <c r="I36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J36">
-        <v>8.6515258995131786E-5</v>
+        <v>9.0519475170192248E-5</v>
       </c>
       <c r="M36" t="s">
         <v>14</v>
       </c>
       <c r="N36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O36">
         <v>0</v>
@@ -7023,16 +7023,16 @@
         <v>295</v>
       </c>
       <c r="I37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J37">
-        <v>8.6515258995131786E-5</v>
+        <v>8.5315524965969179E-5</v>
       </c>
       <c r="M37" t="s">
         <v>14</v>
       </c>
       <c r="N37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O37">
         <v>0</v>
@@ -7055,16 +7055,16 @@
         <v>295</v>
       </c>
       <c r="I38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J38">
-        <v>8.6903540043735565E-5</v>
+        <v>8.3659722628261828E-5</v>
       </c>
       <c r="M38" t="s">
         <v>14</v>
       </c>
       <c r="N38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O38">
         <v>0</v>
@@ -7087,16 +7087,16 @@
         <v>295</v>
       </c>
       <c r="I39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J39">
-        <v>9.2288998187870096E-5</v>
+        <v>8.3659722628261828E-5</v>
       </c>
       <c r="M39" t="s">
         <v>14</v>
       </c>
       <c r="N39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O39">
         <v>0</v>
@@ -7119,16 +7119,16 @@
         <v>295</v>
       </c>
       <c r="I40" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J40">
-        <v>1.0194554786664628E-4</v>
+        <v>8.4035188010961892E-5</v>
       </c>
       <c r="M40" t="s">
         <v>14</v>
       </c>
       <c r="N40" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O40">
         <v>0</v>
@@ -7151,16 +7151,16 @@
         <v>295</v>
       </c>
       <c r="I41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J41">
-        <v>1.1266987042908288E-4</v>
+        <v>8.9242892869011972E-5</v>
       </c>
       <c r="M41" t="s">
         <v>14</v>
       </c>
       <c r="N41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O41">
         <v>0</v>
@@ -7183,16 +7183,16 @@
         <v>295</v>
       </c>
       <c r="I42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J42">
-        <v>1.2344078671735191E-4</v>
+        <v>9.8580716936762895E-5</v>
       </c>
       <c r="M42" t="s">
         <v>14</v>
       </c>
       <c r="N42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="O42">
         <v>0</v>
@@ -7215,16 +7215,16 @@
         <v>295</v>
       </c>
       <c r="I43" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J43">
-        <v>1.286981121154472E-4</v>
+        <v>1.0895107080693903E-4</v>
       </c>
       <c r="M43" t="s">
         <v>14</v>
       </c>
       <c r="N43" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O43">
         <v>0</v>
@@ -7247,16 +7247,16 @@
         <v>295</v>
       </c>
       <c r="I44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J44">
-        <v>1.2912910407939738E-4</v>
+        <v>1.1936648052303917E-4</v>
       </c>
       <c r="M44" t="s">
         <v>14</v>
       </c>
       <c r="N44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O44">
         <v>0</v>
@@ -7279,16 +7279,16 @@
         <v>295</v>
       </c>
       <c r="I45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J45">
-        <v>1.2923782277300645E-4</v>
+        <v>1.2445028180479821E-4</v>
       </c>
       <c r="M45" t="s">
         <v>14</v>
       </c>
       <c r="N45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O45">
         <v>0</v>
@@ -7311,16 +7311,16 @@
         <v>295</v>
       </c>
       <c r="I46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J46">
-        <v>1.2908251035356492E-4</v>
+        <v>1.248670483795953E-4</v>
       </c>
       <c r="M46" t="s">
         <v>14</v>
       </c>
       <c r="N46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O46">
         <v>0</v>
@@ -7343,16 +7343,16 @@
         <v>295</v>
       </c>
       <c r="I47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J47">
-        <v>1.2932712741418531E-4</v>
+        <v>1.2497217868675132E-4</v>
       </c>
       <c r="M47" t="s">
         <v>14</v>
       </c>
       <c r="N47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O47">
         <v>0</v>
@@ -7375,16 +7375,16 @@
         <v>295</v>
       </c>
       <c r="I48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J48">
-        <v>1.2889613545023513E-4</v>
+        <v>1.2482199253367128E-4</v>
       </c>
       <c r="M48" t="s">
         <v>14</v>
       </c>
       <c r="N48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O48">
         <v>0</v>
@@ -7407,16 +7407,16 @@
         <v>295</v>
       </c>
       <c r="I49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J49">
-        <v>1.285272684540615E-4</v>
+        <v>1.2505853572477232E-4</v>
       </c>
       <c r="M49" t="s">
         <v>14</v>
       </c>
       <c r="N49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O49">
         <v>0</v>
@@ -7439,16 +7439,16 @@
         <v>295</v>
       </c>
       <c r="I50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J50">
-        <v>1.2846902629677095E-4</v>
+        <v>1.2464176914997525E-4</v>
       </c>
       <c r="M50" t="s">
         <v>14</v>
       </c>
       <c r="N50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O50">
         <v>0</v>
@@ -7471,16 +7471,16 @@
         <v>295</v>
       </c>
       <c r="I51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J51">
-        <v>1.2880294799857021E-4</v>
+        <v>1.2428507703641018E-4</v>
       </c>
       <c r="M51" t="s">
         <v>14</v>
       </c>
       <c r="N51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O51">
         <v>0</v>
@@ -7503,16 +7503,16 @@
         <v>295</v>
       </c>
       <c r="I52" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J52">
-        <v>1.2848067472822906E-4</v>
+        <v>1.2422875722900518E-4</v>
       </c>
       <c r="M52" t="s">
         <v>14</v>
       </c>
       <c r="N52" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O52">
         <v>0</v>
@@ -7535,16 +7535,16 @@
         <v>295</v>
       </c>
       <c r="I53" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J53">
-        <v>1.2881847924051435E-4</v>
+        <v>1.2455165745812723E-4</v>
       </c>
       <c r="M53" t="s">
         <v>14</v>
       </c>
       <c r="N53" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O53">
         <v>0</v>
@@ -7567,16 +7567,16 @@
         <v>295</v>
       </c>
       <c r="I54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J54">
-        <v>1.277973000826864E-4</v>
+        <v>1.2424002119048615E-4</v>
       </c>
       <c r="M54" t="s">
         <v>14</v>
       </c>
       <c r="N54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O54">
         <v>0</v>
@@ -7599,16 +7599,16 @@
         <v>295</v>
       </c>
       <c r="I55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J55">
-        <v>1.2460562986316327E-4</v>
+        <v>1.2456667607343522E-4</v>
       </c>
       <c r="M55" t="s">
         <v>14</v>
       </c>
       <c r="N55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O55">
         <v>0</v>
@@ -7631,16 +7631,16 @@
         <v>295</v>
       </c>
       <c r="I56" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J56">
-        <v>1.1839701589598872E-4</v>
+        <v>1.2357920211693405E-4</v>
       </c>
       <c r="M56" t="s">
         <v>14</v>
       </c>
       <c r="N56" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O56">
         <v>0</v>
@@ -7663,16 +7663,16 @@
         <v>295</v>
       </c>
       <c r="I57" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J57">
-        <v>1.0072634537403038E-4</v>
+        <v>1.2049287667113939E-4</v>
       </c>
       <c r="M57" t="s">
         <v>14</v>
       </c>
       <c r="N57" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O57">
         <v>0</v>
@@ -7695,16 +7695,16 @@
         <v>295</v>
       </c>
       <c r="I58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J58">
-        <v>9.3352888261044467E-5</v>
+        <v>1.1448918520176516E-4</v>
       </c>
       <c r="M58" t="s">
         <v>14</v>
       </c>
       <c r="N58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O58">
         <v>0</v>
@@ -7727,19 +7727,19 @@
         <v>295</v>
       </c>
       <c r="I59" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J59">
-        <v>0.16586017091895719</v>
+        <v>9.7401755635084653E-5</v>
       </c>
       <c r="M59" t="s">
         <v>14</v>
       </c>
       <c r="N59" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="O59">
-        <v>0.10058384047674074</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.45">
@@ -7759,19 +7759,19 @@
         <v>295</v>
       </c>
       <c r="I60" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J60">
-        <v>7.4477131881831887E-2</v>
+        <v>9.0271668017610185E-5</v>
       </c>
       <c r="M60" t="s">
         <v>14</v>
       </c>
       <c r="N60" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O60">
-        <v>0.21509120647864077</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.45">
@@ -7791,19 +7791,19 @@
         <v>295</v>
       </c>
       <c r="I61" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J61">
-        <v>2.514750562927762E-2</v>
+        <v>0.15730252843276799</v>
       </c>
       <c r="M61" t="s">
         <v>14</v>
       </c>
       <c r="N61" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O61">
-        <v>7.1165977183329288E-2</v>
+        <v>0.11846397239250783</v>
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.45">
@@ -7823,19 +7823,19 @@
         <v>295</v>
       </c>
       <c r="I62" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J62">
-        <v>9.3012589732482056E-5</v>
+        <v>8.2099008544369065E-2</v>
       </c>
       <c r="M62" t="s">
         <v>14</v>
       </c>
       <c r="N62" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="O62">
-        <v>0</v>
+        <v>0.25517110207600147</v>
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.45">
@@ -7855,19 +7855,19 @@
         <v>295</v>
       </c>
       <c r="I63" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J63">
-        <v>9.1762324755977867E-5</v>
+        <v>2.5656659203133272E-2</v>
       </c>
       <c r="M63" t="s">
         <v>14</v>
       </c>
       <c r="N63" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="O63">
-        <v>0</v>
+        <v>6.4509870400166092E-2</v>
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.45">
@@ -7887,16 +7887,16 @@
         <v>295</v>
       </c>
       <c r="I64" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J64">
-        <v>9.1762324755977867E-5</v>
+        <v>9.4418148798065913E-5</v>
       </c>
       <c r="M64" t="s">
         <v>14</v>
       </c>
       <c r="N64" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="O64">
         <v>0</v>
@@ -7919,16 +7919,16 @@
         <v>295</v>
       </c>
       <c r="I65" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J65">
-        <v>9.7140017279140312E-5</v>
+        <v>8.9942601436281E-5</v>
       </c>
       <c r="M65" t="s">
         <v>14</v>
       </c>
       <c r="N65" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O65">
         <v>0</v>
@@ -7951,16 +7951,16 @@
         <v>295</v>
       </c>
       <c r="I66" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J66">
-        <v>1.1874785763394104E-4</v>
+        <v>8.8733602903986751E-5</v>
       </c>
       <c r="M66" t="s">
         <v>14</v>
       </c>
       <c r="N66" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="O66">
         <v>0</v>
@@ -7983,16 +7983,16 @@
         <v>295</v>
       </c>
       <c r="I67" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J67">
-        <v>1.3623991887354165E-4</v>
+        <v>8.8733602903986751E-5</v>
       </c>
       <c r="M67" t="s">
         <v>14</v>
       </c>
       <c r="N67" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="O67">
         <v>0</v>
@@ -8015,16 +8015,16 @@
         <v>295</v>
       </c>
       <c r="I68" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J68">
-        <v>1.4843194379970056E-4</v>
+        <v>9.3933798454382821E-5</v>
       </c>
       <c r="M68" t="s">
         <v>14</v>
       </c>
       <c r="N68" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O68">
         <v>0</v>
@@ -8047,16 +8047,16 @@
         <v>295</v>
       </c>
       <c r="I69" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J69">
-        <v>1.5452407345229396E-4</v>
+        <v>1.1482844700164211E-4</v>
       </c>
       <c r="M69" t="s">
         <v>14</v>
       </c>
       <c r="N69" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="O69">
         <v>0</v>
@@ -8079,16 +8079,16 @@
         <v>295</v>
       </c>
       <c r="I70" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J70">
-        <v>1.5527733868658531E-4</v>
+        <v>1.3174316249228059E-4</v>
       </c>
       <c r="M70" t="s">
         <v>14</v>
       </c>
       <c r="N70" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O70">
         <v>0</v>
@@ -8111,16 +8111,16 @@
         <v>295</v>
       </c>
       <c r="I71" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J71">
-        <v>1.5489294044846756E-4</v>
+        <v>1.4353277550906298E-4</v>
       </c>
       <c r="M71" t="s">
         <v>14</v>
       </c>
       <c r="N71" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O71">
         <v>0</v>
@@ -8143,16 +8143,16 @@
         <v>295</v>
       </c>
       <c r="I72" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J72">
-        <v>1.5489294044846756E-4</v>
+        <v>1.4942382736362722E-4</v>
       </c>
       <c r="M72" t="s">
         <v>14</v>
       </c>
       <c r="N72" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="O72">
         <v>0</v>
@@ -8175,16 +8175,16 @@
         <v>295</v>
       </c>
       <c r="I73" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J73">
-        <v>1.5477645613388641E-4</v>
+        <v>1.5015223020606536E-4</v>
       </c>
       <c r="M73" t="s">
         <v>14</v>
       </c>
       <c r="N73" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="O73">
         <v>0</v>
@@ -8207,16 +8207,16 @@
         <v>295</v>
       </c>
       <c r="I74" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J74">
-        <v>1.5477645613388641E-4</v>
+        <v>1.4978051947719229E-4</v>
       </c>
       <c r="M74" t="s">
         <v>14</v>
       </c>
       <c r="N74" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O74">
         <v>0</v>
@@ -8239,16 +8239,16 @@
         <v>295</v>
       </c>
       <c r="I75" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J75">
-        <v>1.546133780934728E-4</v>
+        <v>1.4978051947719229E-4</v>
       </c>
       <c r="M75" t="s">
         <v>14</v>
       </c>
       <c r="N75" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="O75">
         <v>0</v>
@@ -8271,16 +8271,16 @@
         <v>295</v>
       </c>
       <c r="I76" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J76">
-        <v>1.546133780934728E-4</v>
+        <v>1.4966787986238225E-4</v>
       </c>
       <c r="M76" t="s">
         <v>14</v>
       </c>
       <c r="N76" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="O76">
         <v>0</v>
@@ -8303,16 +8303,16 @@
         <v>295</v>
       </c>
       <c r="I77" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J77">
-        <v>1.5839911831735972E-4</v>
+        <v>1.4966787986238225E-4</v>
       </c>
       <c r="M77" t="s">
         <v>14</v>
       </c>
       <c r="N77" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="O77">
         <v>0</v>
@@ -8335,16 +8335,16 @@
         <v>295</v>
       </c>
       <c r="I78" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J78">
-        <v>1.5883011028130993E-4</v>
+        <v>1.4951018440164822E-4</v>
       </c>
       <c r="M78" t="s">
         <v>14</v>
       </c>
       <c r="N78" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O78">
         <v>0</v>
@@ -8367,16 +8367,16 @@
         <v>295</v>
       </c>
       <c r="I79" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J79">
-        <v>1.5883011028130996E-4</v>
+        <v>1.4951018440164822E-4</v>
       </c>
       <c r="M79" t="s">
         <v>14</v>
       </c>
       <c r="N79" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="O79">
         <v>0</v>
@@ -8399,16 +8399,16 @@
         <v>295</v>
       </c>
       <c r="I80" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J80">
-        <v>1.5378245664946072E-4</v>
+        <v>1.5317097188297397E-4</v>
       </c>
       <c r="M80" t="s">
         <v>14</v>
       </c>
       <c r="N80" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="O80">
         <v>0</v>
@@ -8431,16 +8431,16 @@
         <v>295</v>
       </c>
       <c r="I81" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J81">
-        <v>1.4145453335629048E-4</v>
+        <v>1.5358773845777109E-4</v>
       </c>
       <c r="M81" t="s">
         <v>14</v>
       </c>
       <c r="N81" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="O81">
         <v>0</v>
@@ -8463,16 +8463,16 @@
         <v>295</v>
       </c>
       <c r="I82" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J82">
-        <v>1.342985136305227E-4</v>
+        <v>1.5358773845777109E-4</v>
       </c>
       <c r="M82" t="s">
         <v>14</v>
       </c>
       <c r="N82" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="O82">
         <v>0</v>
@@ -8495,16 +8495,16 @@
         <v>295</v>
       </c>
       <c r="I83" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J83">
-        <v>1.2523603395611031E-4</v>
+        <v>1.4870668848267007E-4</v>
       </c>
       <c r="M83" t="s">
         <v>14</v>
       </c>
       <c r="N83" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="O83">
         <v>0</v>
@@ -8527,16 +8527,16 @@
         <v>295</v>
       </c>
       <c r="I84" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J84">
-        <v>1.0476197426323264E-4</v>
+        <v>1.3678566258194263E-4</v>
       </c>
       <c r="M84" t="s">
         <v>14</v>
       </c>
       <c r="N84" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="O84">
         <v>0</v>
@@ -8559,16 +8559,16 @@
         <v>295</v>
       </c>
       <c r="I85" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J85">
-        <v>9.3024238163940171E-5</v>
+        <v>1.2986583557878019E-4</v>
       </c>
       <c r="M85" t="s">
         <v>14</v>
       </c>
       <c r="N85" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="O85">
         <v>0</v>
@@ -8591,16 +8591,16 @@
         <v>295</v>
       </c>
       <c r="I86" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="J86">
-        <v>9.1773973187435969E-5</v>
+        <v>1.211024735465604E-4</v>
       </c>
       <c r="M86" t="s">
         <v>14</v>
       </c>
       <c r="N86" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="O86">
         <v>0</v>
@@ -8623,16 +8623,16 @@
         <v>295</v>
       </c>
       <c r="I87" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J87">
-        <v>9.1773973187435969E-5</v>
+        <v>1.0130418391678533E-4</v>
       </c>
       <c r="M87" t="s">
         <v>14</v>
       </c>
       <c r="N87" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="O87">
         <v>0</v>
@@ -8655,16 +8655,16 @@
         <v>295</v>
       </c>
       <c r="I88" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J88">
-        <v>9.7151665710598414E-5</v>
+        <v>9.4947554987673017E-5</v>
       </c>
       <c r="M88" t="s">
         <v>14</v>
       </c>
       <c r="N88" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="O88">
         <v>0</v>
@@ -8687,16 +8687,16 @@
         <v>295</v>
       </c>
       <c r="I89" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="J89">
-        <v>1.1959431031989731E-4</v>
+        <v>8.9953865397762007E-5</v>
       </c>
       <c r="M89" t="s">
         <v>14</v>
       </c>
       <c r="N89" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="O89">
         <v>0</v>
@@ -8719,16 +8719,16 @@
         <v>295</v>
       </c>
       <c r="I90" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J90">
-        <v>1.3757948849122472E-4</v>
+        <v>8.8744866865467757E-5</v>
       </c>
       <c r="M90" t="s">
         <v>14</v>
       </c>
       <c r="N90" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="O90">
         <v>0</v>
@@ -8751,16 +8751,16 @@
         <v>295</v>
       </c>
       <c r="I91" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="J91">
-        <v>1.4843194379970056E-4</v>
+        <v>8.8744866865467757E-5</v>
       </c>
       <c r="M91" t="s">
         <v>14</v>
       </c>
       <c r="N91" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="O91">
         <v>0</v>
@@ -8783,16 +8783,16 @@
         <v>295</v>
       </c>
       <c r="I92" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="J92">
-        <v>1.5320003507655503E-4</v>
+        <v>9.3945062415863814E-5</v>
       </c>
       <c r="M92" t="s">
         <v>14</v>
       </c>
       <c r="N92" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="O92">
         <v>0</v>
@@ -8815,16 +8815,16 @@
         <v>295</v>
       </c>
       <c r="I93" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="J93">
-        <v>1.5470268273465166E-4</v>
+        <v>1.1564696153592828E-4</v>
       </c>
       <c r="M93" t="s">
         <v>14</v>
       </c>
       <c r="N93" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="O93">
         <v>0</v>
@@ -8847,16 +8847,16 @@
         <v>295</v>
       </c>
       <c r="I94" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J94">
-        <v>1.5385623004869544E-4</v>
+        <v>1.3303851806259584E-4</v>
       </c>
       <c r="M94" t="s">
         <v>14</v>
       </c>
       <c r="N94" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="O94">
         <v>0</v>
@@ -8879,16 +8879,16 @@
         <v>295</v>
       </c>
       <c r="I95" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="J95">
-        <v>1.5297871487885087E-4</v>
+        <v>1.4353277550906301E-4</v>
       </c>
       <c r="M95" t="s">
         <v>14</v>
       </c>
       <c r="N95" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="O95">
         <v>0</v>
@@ -8911,16 +8911,16 @@
         <v>295</v>
       </c>
       <c r="I96" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J96">
-        <v>1.5178669205963724E-4</v>
+        <v>1.4814349040861996E-4</v>
       </c>
       <c r="M96" t="s">
         <v>14</v>
       </c>
       <c r="N96" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="O96">
         <v>0</v>
@@ -8943,16 +8943,16 @@
         <v>295</v>
       </c>
       <c r="I97" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J97">
-        <v>1.511965048657595E-4</v>
+        <v>1.4959654143966924E-4</v>
       </c>
       <c r="M97" t="s">
         <v>14</v>
       </c>
       <c r="N97" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="O97">
         <v>0</v>
@@ -8975,16 +8975,16 @@
         <v>295</v>
       </c>
       <c r="I98" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J98">
-        <v>1.5102954401485986E-4</v>
+        <v>1.4877802690538308E-4</v>
       </c>
       <c r="M98" t="s">
         <v>14</v>
       </c>
       <c r="N98" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O98">
         <v>0</v>
@@ -9007,16 +9007,16 @@
         <v>295</v>
       </c>
       <c r="I99" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="J99">
-        <v>1.5162361401922369E-4</v>
+        <v>1.479294751404809E-4</v>
       </c>
       <c r="M99" t="s">
         <v>14</v>
       </c>
       <c r="N99" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="O99">
         <v>0</v>
@@ -9039,16 +9039,16 @@
         <v>295</v>
       </c>
       <c r="I100" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="J100">
-        <v>1.5817779811965561E-4</v>
+        <v>1.4677679641559167E-4</v>
       </c>
       <c r="M100" t="s">
         <v>14</v>
       </c>
       <c r="N100" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="O100">
         <v>0</v>
@@ -9071,16 +9071,16 @@
         <v>295</v>
       </c>
       <c r="I101" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="J101">
-        <v>1.5883011028130993E-4</v>
+        <v>1.4620608903388756E-4</v>
       </c>
       <c r="M101" t="s">
         <v>14</v>
       </c>
       <c r="N101" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="O101">
         <v>0</v>
@@ -9103,16 +9103,16 @@
         <v>295</v>
       </c>
       <c r="I102" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="J102">
-        <v>1.5995612532226092E-4</v>
+        <v>1.460446389193265E-4</v>
       </c>
       <c r="M102" t="s">
         <v>14</v>
       </c>
       <c r="N102" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="O102">
         <v>0</v>
@@ -9135,16 +9135,16 @@
         <v>295</v>
       </c>
       <c r="I103" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J103">
-        <v>1.5438817508528263E-4</v>
+        <v>1.4661910095485763E-4</v>
       </c>
       <c r="M103" t="s">
         <v>14</v>
       </c>
       <c r="N103" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="O103">
         <v>0</v>
@@ -9167,16 +9167,16 @@
         <v>295</v>
       </c>
       <c r="I104" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="J104">
-        <v>1.4110508041254708E-4</v>
+        <v>1.5295695661483494E-4</v>
       </c>
       <c r="M104" t="s">
         <v>14</v>
       </c>
       <c r="N104" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="O104">
         <v>0</v>
@@ -9199,16 +9199,16 @@
         <v>295</v>
       </c>
       <c r="I105" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J105">
-        <v>1.3460137284843364E-4</v>
+        <v>1.5358773845777109E-4</v>
       </c>
       <c r="M105" t="s">
         <v>14</v>
       </c>
       <c r="N105" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="O105">
         <v>0</v>
@@ -9231,16 +9231,16 @@
         <v>295</v>
       </c>
       <c r="I106" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J106">
-        <v>1.2500306532694806E-4</v>
+        <v>1.5467658806760128E-4</v>
       </c>
       <c r="M106" t="s">
         <v>14</v>
       </c>
       <c r="N106" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="O106">
         <v>0</v>
@@ -9263,16 +9263,16 @@
         <v>295</v>
       </c>
       <c r="I107" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="J107">
-        <v>1.0499106008190886E-4</v>
+        <v>1.4929241447968219E-4</v>
       </c>
       <c r="M107" t="s">
         <v>14</v>
       </c>
       <c r="N107" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="O107">
         <v>0</v>
@@ -9292,13 +9292,22 @@
         <v>291</v>
       </c>
       <c r="H108" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I108" t="s">
-        <v>178</v>
+        <v>284</v>
       </c>
       <c r="J108">
-        <v>0.14340008535826368</v>
+        <v>1.3644774373751257E-4</v>
+      </c>
+      <c r="M108" t="s">
+        <v>14</v>
+      </c>
+      <c r="N108" t="s">
+        <v>284</v>
+      </c>
+      <c r="O108">
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.45">
@@ -9315,13 +9324,22 @@
         <v>291</v>
       </c>
       <c r="H109" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I109" t="s">
-        <v>181</v>
+        <v>285</v>
       </c>
       <c r="J109">
-        <v>8.6521998749355733E-2</v>
+        <v>1.3015869857728625E-4</v>
+      </c>
+      <c r="M109" t="s">
+        <v>14</v>
+      </c>
+      <c r="N109" t="s">
+        <v>285</v>
+      </c>
+      <c r="O109">
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.45">
@@ -9338,13 +9356,22 @@
         <v>291</v>
       </c>
       <c r="H110" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I110" t="s">
-        <v>182</v>
+        <v>286</v>
       </c>
       <c r="J110">
-        <v>2.2066632048695019E-2</v>
+        <v>1.2087719431694036E-4</v>
+      </c>
+      <c r="M110" t="s">
+        <v>14</v>
+      </c>
+      <c r="N110" t="s">
+        <v>286</v>
+      </c>
+      <c r="O110">
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.45">
@@ -9361,13 +9388,22 @@
         <v>291</v>
       </c>
       <c r="H111" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I111" t="s">
-        <v>183</v>
+        <v>287</v>
       </c>
       <c r="J111">
-        <v>0.14334882658191628</v>
+        <v>1.0152570849257837E-4</v>
+      </c>
+      <c r="M111" t="s">
+        <v>14</v>
+      </c>
+      <c r="N111" t="s">
+        <v>287</v>
+      </c>
+      <c r="O111">
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.45">
@@ -9375,10 +9411,10 @@
         <v>296</v>
       </c>
       <c r="I112" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="J112">
-        <v>8.6598587527055154E-2</v>
+        <v>0.13731773220396418</v>
       </c>
     </row>
     <row r="113" spans="8:10" x14ac:dyDescent="0.45">
@@ -9386,10 +9422,10 @@
         <v>296</v>
       </c>
       <c r="I113" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J113">
-        <v>2.2037352629910668E-2</v>
+        <v>9.3476795402542598E-2</v>
       </c>
     </row>
     <row r="114" spans="8:10" x14ac:dyDescent="0.45">
@@ -9397,10 +9433,10 @@
         <v>296</v>
       </c>
       <c r="I114" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="J114">
-        <v>0.13859280204946153</v>
+        <v>2.1204264978092399E-2</v>
       </c>
     </row>
     <row r="115" spans="8:10" x14ac:dyDescent="0.45">
@@ -9408,10 +9444,10 @@
         <v>296</v>
       </c>
       <c r="I115" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="J115">
-        <v>8.3772085498839563E-2</v>
+        <v>0.13726428706211127</v>
       </c>
     </row>
     <row r="116" spans="8:10" x14ac:dyDescent="0.45">
@@ -9419,10 +9455,10 @@
         <v>296</v>
       </c>
       <c r="I116" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J116">
-        <v>2.1344084636896916E-2</v>
+        <v>9.3581280710609713E-2</v>
       </c>
     </row>
     <row r="117" spans="8:10" x14ac:dyDescent="0.45">
@@ -9430,10 +9466,10 @@
         <v>296</v>
       </c>
       <c r="I117" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="J117">
-        <v>1.1705797645924358E-4</v>
+        <v>2.1159485355029328E-2</v>
       </c>
     </row>
     <row r="118" spans="8:10" x14ac:dyDescent="0.45">
@@ -9441,10 +9477,10 @@
         <v>296</v>
       </c>
       <c r="I118" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="J118">
-        <v>1.1705797645924358E-4</v>
+        <v>0.13271145679875751</v>
       </c>
     </row>
     <row r="119" spans="8:10" x14ac:dyDescent="0.45">
@@ -9452,10 +9488,10 @@
         <v>296</v>
       </c>
       <c r="I119" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="J119">
-        <v>1.1708927977011483E-4</v>
+        <v>9.0527689906246239E-2</v>
       </c>
     </row>
     <row r="120" spans="8:10" x14ac:dyDescent="0.45">
@@ -9463,10 +9499,10 @@
         <v>296</v>
       </c>
       <c r="I120" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J120">
-        <v>1.1752345669189907E-4</v>
+        <v>2.0493404929269193E-2</v>
       </c>
     </row>
     <row r="121" spans="8:10" x14ac:dyDescent="0.45">
@@ -9474,10 +9510,10 @@
         <v>296</v>
       </c>
       <c r="I121" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="J121">
-        <v>1.1830197003326707E-4</v>
+        <v>1.1239100775724166E-4</v>
       </c>
     </row>
     <row r="122" spans="8:10" x14ac:dyDescent="0.45">
@@ -9485,10 +9521,10 @@
         <v>296</v>
       </c>
       <c r="I122" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="J122">
-        <v>1.1916656747953098E-4</v>
+        <v>1.1226161861562765E-4</v>
       </c>
     </row>
     <row r="123" spans="8:10" x14ac:dyDescent="0.45">
@@ -9496,10 +9532,10 @@
         <v>296</v>
       </c>
       <c r="I123" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="J123">
-        <v>1.1997450593311794E-4</v>
+        <v>1.1226161861562765E-4</v>
       </c>
     </row>
     <row r="124" spans="8:10" x14ac:dyDescent="0.45">
@@ -9507,10 +9543,10 @@
         <v>296</v>
       </c>
       <c r="I124" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="J124">
-        <v>1.2043529066914273E-4</v>
+        <v>1.122916392981367E-4</v>
       </c>
     </row>
     <row r="125" spans="8:10" x14ac:dyDescent="0.45">
@@ -9518,10 +9554,10 @@
         <v>296</v>
       </c>
       <c r="I125" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="J125">
-        <v>1.2046095938405716E-4</v>
+        <v>1.127080261645372E-4</v>
       </c>
     </row>
     <row r="126" spans="8:10" x14ac:dyDescent="0.45">
@@ -9529,10 +9565,10 @@
         <v>296</v>
       </c>
       <c r="I126" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="J126">
-        <v>1.2047222857597082E-4</v>
+        <v>1.1345464053853728E-4</v>
       </c>
     </row>
     <row r="127" spans="8:10" x14ac:dyDescent="0.45">
@@ -9540,10 +9576,10 @@
         <v>296</v>
       </c>
       <c r="I127" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="J127">
-        <v>1.2047379374151438E-4</v>
+        <v>1.1428381178943722E-4</v>
       </c>
     </row>
     <row r="128" spans="8:10" x14ac:dyDescent="0.45">
@@ -9551,10 +9587,10 @@
         <v>296</v>
       </c>
       <c r="I128" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="J128">
-        <v>1.2048255866855832E-4</v>
+        <v>1.1505864560499576E-4</v>
       </c>
     </row>
     <row r="129" spans="8:10" x14ac:dyDescent="0.45">
@@ -9562,10 +9598,10 @@
         <v>296</v>
       </c>
       <c r="I129" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="J129">
-        <v>1.2045782905297005E-4</v>
+        <v>1.1550055005152896E-4</v>
       </c>
     </row>
     <row r="130" spans="8:10" x14ac:dyDescent="0.45">
@@ -9573,10 +9609,10 @@
         <v>296</v>
       </c>
       <c r="I130" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="J130">
-        <v>1.2043748190090373E-4</v>
+        <v>1.1552516701118639E-4</v>
       </c>
     </row>
     <row r="131" spans="8:10" x14ac:dyDescent="0.45">
@@ -9584,10 +9620,10 @@
         <v>296</v>
       </c>
       <c r="I131" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="J131">
-        <v>1.2043278640427306E-4</v>
+        <v>1.1553597445688965E-4</v>
       </c>
     </row>
     <row r="132" spans="8:10" x14ac:dyDescent="0.45">
@@ -9595,10 +9631,10 @@
         <v>296</v>
       </c>
       <c r="I132" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J132">
-        <v>1.2046722004623141E-4</v>
+        <v>1.1553747549101509E-4</v>
       </c>
     </row>
     <row r="133" spans="8:10" x14ac:dyDescent="0.45">
@@ -9606,10 +9642,10 @@
         <v>296</v>
       </c>
       <c r="I133" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="J133">
-        <v>1.2044123829820828E-4</v>
+        <v>1.1554588128211763E-4</v>
       </c>
     </row>
     <row r="134" spans="8:10" x14ac:dyDescent="0.45">
@@ -9617,10 +9653,10 @@
         <v>296</v>
       </c>
       <c r="I134" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="J134">
-        <v>1.204769240726015E-4</v>
+        <v>1.1552216494293549E-4</v>
       </c>
     </row>
     <row r="135" spans="8:10" x14ac:dyDescent="0.45">
@@ -9628,10 +9664,10 @@
         <v>296</v>
       </c>
       <c r="I135" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="J135">
-        <v>1.2038614447107488E-4</v>
+        <v>1.155026514993046E-4</v>
       </c>
     </row>
     <row r="136" spans="8:10" x14ac:dyDescent="0.45">
@@ -9639,10 +9675,10 @@
         <v>296</v>
       </c>
       <c r="I136" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="J136">
-        <v>1.201288312557132E-4</v>
+        <v>1.1549814839692826E-4</v>
       </c>
     </row>
     <row r="137" spans="8:10" x14ac:dyDescent="0.45">
@@ -9650,10 +9686,10 @@
         <v>296</v>
       </c>
       <c r="I137" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="J137">
-        <v>1.1963173467907775E-4</v>
+        <v>1.1553117114768819E-4</v>
       </c>
     </row>
     <row r="138" spans="8:10" x14ac:dyDescent="0.45">
@@ -9661,10 +9697,10 @@
         <v>296</v>
       </c>
       <c r="I138" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="J138">
-        <v>1.1822402478919763E-4</v>
+        <v>1.1550625398120568E-4</v>
       </c>
     </row>
     <row r="139" spans="8:10" x14ac:dyDescent="0.45">
@@ -9672,10 +9708,10 @@
         <v>296</v>
       </c>
       <c r="I139" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J139">
-        <v>1.1762988794886131E-4</v>
+        <v>1.1554047755926599E-4</v>
       </c>
     </row>
     <row r="140" spans="8:10" x14ac:dyDescent="0.45">
@@ -9683,10 +9719,10 @@
         <v>296</v>
       </c>
       <c r="I140" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="J140">
-        <v>1.1705797645924357E-4</v>
+        <v>1.1545341757998976E-4</v>
       </c>
     </row>
     <row r="141" spans="8:10" x14ac:dyDescent="0.45">
@@ -9694,10 +9730,10 @@
         <v>296</v>
       </c>
       <c r="I141" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="J141">
-        <v>1.1705797645924357E-4</v>
+        <v>1.1520664756976537E-4</v>
       </c>
     </row>
     <row r="142" spans="8:10" x14ac:dyDescent="0.45">
@@ -9705,10 +9741,10 @@
         <v>296</v>
       </c>
       <c r="I142" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="J142">
-        <v>1.1708927977011482E-4</v>
+        <v>1.1472991913152167E-4</v>
       </c>
     </row>
     <row r="143" spans="8:10" x14ac:dyDescent="0.45">
@@ -9716,10 +9752,10 @@
         <v>296</v>
       </c>
       <c r="I143" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="J143">
-        <v>1.1752345669189907E-4</v>
+        <v>1.1337988903908973E-4</v>
       </c>
     </row>
     <row r="144" spans="8:10" x14ac:dyDescent="0.45">
@@ -9727,10 +9763,10 @@
         <v>296</v>
       </c>
       <c r="I144" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="J144">
-        <v>1.1830197003326704E-4</v>
+        <v>1.1281009648506798E-4</v>
       </c>
     </row>
     <row r="145" spans="8:10" x14ac:dyDescent="0.45">
@@ -9738,10 +9774,10 @@
         <v>296</v>
       </c>
       <c r="I145" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="J145">
-        <v>1.1916656747953097E-4</v>
+        <v>1.1239400982549256E-4</v>
       </c>
     </row>
     <row r="146" spans="8:10" x14ac:dyDescent="0.45">
@@ -9749,10 +9785,10 @@
         <v>296</v>
       </c>
       <c r="I146" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="J146">
-        <v>1.2003492132309945E-4</v>
+        <v>1.1226161861562765E-4</v>
       </c>
     </row>
     <row r="147" spans="8:10" x14ac:dyDescent="0.45">
@@ -9760,10 +9796,10 @@
         <v>296</v>
       </c>
       <c r="I147" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="J147">
-        <v>1.2045876815229618E-4</v>
+        <v>1.1226161861562765E-4</v>
       </c>
     </row>
     <row r="148" spans="8:10" x14ac:dyDescent="0.45">
@@ -9771,10 +9807,10 @@
         <v>296</v>
       </c>
       <c r="I148" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="J148">
-        <v>1.2049351482736326E-4</v>
+        <v>1.1229163929813669E-4</v>
       </c>
     </row>
     <row r="149" spans="8:10" x14ac:dyDescent="0.45">
@@ -9782,10 +9818,10 @@
         <v>296</v>
       </c>
       <c r="I149" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J149">
-        <v>1.205022797544072E-4</v>
+        <v>1.127080261645372E-4</v>
       </c>
     </row>
     <row r="150" spans="8:10" x14ac:dyDescent="0.45">
@@ -9793,10 +9829,10 @@
         <v>296</v>
       </c>
       <c r="I150" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="J150">
-        <v>1.2048975843005872E-4</v>
+        <v>1.1345464053853725E-4</v>
       </c>
     </row>
     <row r="151" spans="8:10" x14ac:dyDescent="0.45">
@@ -9804,10 +9840,10 @@
         <v>296</v>
       </c>
       <c r="I151" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="J151">
-        <v>1.2050947951590761E-4</v>
+        <v>1.1428381178943719E-4</v>
       </c>
     </row>
     <row r="152" spans="8:10" x14ac:dyDescent="0.45">
@@ -9815,10 +9851,10 @@
         <v>296</v>
       </c>
       <c r="I152" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J152">
-        <v>1.204747328408405E-4</v>
+        <v>1.1511658552223823E-4</v>
       </c>
     </row>
     <row r="153" spans="8:10" x14ac:dyDescent="0.45">
@@ -9826,10 +9862,10 @@
         <v>296</v>
       </c>
       <c r="I153" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J153">
-        <v>1.2044499469551282E-4</v>
+        <v>1.1552306556341075E-4</v>
       </c>
     </row>
     <row r="154" spans="8:10" x14ac:dyDescent="0.45">
@@ -9837,10 +9873,10 @@
         <v>296</v>
       </c>
       <c r="I154" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J154">
-        <v>1.2044029919888212E-4</v>
+        <v>1.1555638852099579E-4</v>
       </c>
     </row>
     <row r="155" spans="8:10" x14ac:dyDescent="0.45">
@@ -9848,10 +9884,10 @@
         <v>296</v>
       </c>
       <c r="I155" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J155">
-        <v>1.2046722004623141E-4</v>
+        <v>1.1556479431209832E-4</v>
       </c>
     </row>
     <row r="156" spans="8:10" x14ac:dyDescent="0.45">
@@ -9859,10 +9895,10 @@
         <v>296</v>
       </c>
       <c r="I156" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="J156">
-        <v>1.2044123829820828E-4</v>
+        <v>1.1555278603909472E-4</v>
       </c>
     </row>
     <row r="157" spans="8:10" x14ac:dyDescent="0.45">
@@ -9870,10 +9906,10 @@
         <v>296</v>
       </c>
       <c r="I157" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="J157">
-        <v>1.2046847217866627E-4</v>
+        <v>1.1557169906907541E-4</v>
       </c>
     </row>
     <row r="158" spans="8:10" x14ac:dyDescent="0.45">
@@ -9881,10 +9917,10 @@
         <v>296</v>
       </c>
       <c r="I158" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="J158">
-        <v>1.2038614447107488E-4</v>
+        <v>1.1553837611149036E-4</v>
       </c>
     </row>
     <row r="159" spans="8:10" x14ac:dyDescent="0.45">
@@ -9892,10 +9928,10 @@
         <v>296</v>
       </c>
       <c r="I159" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="J159">
-        <v>1.201288312557132E-4</v>
+        <v>1.1550985646310676E-4</v>
       </c>
     </row>
     <row r="160" spans="8:10" x14ac:dyDescent="0.45">
@@ -9903,10 +9939,10 @@
         <v>296</v>
       </c>
       <c r="I160" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="J160">
-        <v>1.1962829131488191E-4</v>
+        <v>1.1550535336073039E-4</v>
       </c>
     </row>
     <row r="161" spans="8:10" x14ac:dyDescent="0.45">
@@ -9914,10 +9950,10 @@
         <v>296</v>
       </c>
       <c r="I161" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="J161">
-        <v>1.1820367763713134E-4</v>
+        <v>1.1553117114768819E-4</v>
       </c>
     </row>
     <row r="162" spans="8:10" x14ac:dyDescent="0.45">
@@ -9925,10 +9961,10 @@
         <v>296</v>
       </c>
       <c r="I162" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="J162">
-        <v>1.1760922776368628E-4</v>
+        <v>1.1550625398120568E-4</v>
       </c>
     </row>
     <row r="163" spans="8:10" x14ac:dyDescent="0.45">
@@ -9936,10 +9972,10 @@
         <v>296</v>
       </c>
       <c r="I163" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="J163">
-        <v>0.13767301487845987</v>
+        <v>1.1553237197498855E-4</v>
       </c>
     </row>
     <row r="164" spans="8:10" x14ac:dyDescent="0.45">
@@ -9947,10 +9983,10 @@
         <v>296</v>
       </c>
       <c r="I164" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="J164">
-        <v>8.2497489259150916E-2</v>
+        <v>1.1545341757998976E-4</v>
       </c>
     </row>
     <row r="165" spans="8:10" x14ac:dyDescent="0.45">
@@ -9958,10 +9994,10 @@
         <v>296</v>
       </c>
       <c r="I165" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="J165">
-        <v>2.1150679184671298E-2</v>
+        <v>1.1520664756976537E-4</v>
       </c>
     </row>
     <row r="166" spans="8:10" x14ac:dyDescent="0.45">
@@ -9969,10 +10005,10 @@
         <v>296</v>
       </c>
       <c r="I166" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="J166">
-        <v>1.1608232439584701E-4</v>
+        <v>1.1472661685644568E-4</v>
       </c>
     </row>
     <row r="167" spans="8:10" x14ac:dyDescent="0.45">
@@ -9980,10 +10016,10 @@
         <v>296</v>
       </c>
       <c r="I167" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="J167">
-        <v>1.1598152773484158E-4</v>
+        <v>1.1336037559545885E-4</v>
       </c>
     </row>
     <row r="168" spans="8:10" x14ac:dyDescent="0.45">
@@ -9991,10 +10027,10 @@
         <v>296</v>
       </c>
       <c r="I168" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="J168">
-        <v>1.1598152773484158E-4</v>
+        <v>1.12790282834612E-4</v>
       </c>
     </row>
     <row r="169" spans="8:10" x14ac:dyDescent="0.45">
@@ -10002,10 +10038,10 @@
         <v>296</v>
       </c>
       <c r="I169" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="J169">
-        <v>1.1641507859040841E-4</v>
+        <v>0.13178544922833479</v>
       </c>
     </row>
     <row r="170" spans="8:10" x14ac:dyDescent="0.45">
@@ -10013,10 +10049,10 @@
         <v>296</v>
       </c>
       <c r="I170" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="J170">
-        <v>1.1815710784039348E-4</v>
+        <v>8.9093042175304851E-2</v>
       </c>
     </row>
     <row r="171" spans="8:10" x14ac:dyDescent="0.45">
@@ -10024,10 +10060,10 @@
         <v>296</v>
       </c>
       <c r="I171" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="J171">
-        <v>1.1956732199514328E-4</v>
+        <v>2.0391121930690176E-2</v>
       </c>
     </row>
     <row r="172" spans="8:10" x14ac:dyDescent="0.45">
@@ -10035,10 +10071,10 @@
         <v>296</v>
       </c>
       <c r="I172" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="J172">
-        <v>1.2055024595650054E-4</v>
+        <v>1.1168378965805445E-4</v>
       </c>
     </row>
     <row r="173" spans="8:10" x14ac:dyDescent="0.45">
@@ -10046,10 +10082,10 @@
         <v>296</v>
       </c>
       <c r="I173" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="J173">
-        <v>1.2104139490407044E-4</v>
+        <v>1.1132594312254658E-4</v>
       </c>
     </row>
     <row r="174" spans="8:10" x14ac:dyDescent="0.45">
@@ -10057,10 +10093,10 @@
         <v>296</v>
       </c>
       <c r="I174" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="J174">
-        <v>1.2110212332716067E-4</v>
+        <v>1.1122927652486745E-4</v>
       </c>
     </row>
     <row r="175" spans="8:10" x14ac:dyDescent="0.45">
@@ -10068,10 +10104,10 @@
         <v>296</v>
       </c>
       <c r="I175" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="J175">
-        <v>1.2107113304939813E-4</v>
+        <v>1.1122927652486745E-4</v>
       </c>
     </row>
     <row r="176" spans="8:10" x14ac:dyDescent="0.45">
@@ -10079,10 +10115,10 @@
         <v>296</v>
       </c>
       <c r="I176" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="J176">
-        <v>1.2107113304939813E-4</v>
+        <v>1.1164506297761778E-4</v>
       </c>
     </row>
     <row r="177" spans="8:10" x14ac:dyDescent="0.45">
@@ -10090,10 +10126,10 @@
         <v>296</v>
       </c>
       <c r="I177" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="J177">
-        <v>1.2106174205613676E-4</v>
+        <v>1.1331571395924637E-4</v>
       </c>
     </row>
     <row r="178" spans="8:10" x14ac:dyDescent="0.45">
@@ -10101,10 +10137,10 @@
         <v>296</v>
       </c>
       <c r="I178" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="J178">
-        <v>1.2106174205613676E-4</v>
+        <v>1.1466814570627903E-4</v>
       </c>
     </row>
     <row r="179" spans="8:10" x14ac:dyDescent="0.45">
@@ -10112,10 +10148,10 @@
         <v>296</v>
       </c>
       <c r="I179" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="J179">
-        <v>1.2104859466557084E-4</v>
+        <v>1.1561079513706318E-4</v>
       </c>
     </row>
     <row r="180" spans="8:10" x14ac:dyDescent="0.45">
@@ -10123,10 +10159,10 @@
         <v>296</v>
       </c>
       <c r="I180" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="J180">
-        <v>1.2104859466557084E-4</v>
+        <v>1.1608181964563015E-4</v>
       </c>
     </row>
     <row r="181" spans="8:10" x14ac:dyDescent="0.45">
@@ -10134,10 +10170,10 @@
         <v>296</v>
       </c>
       <c r="I181" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="J181">
-        <v>1.2135380194656553E-4</v>
+        <v>1.161400597696977E-4</v>
       </c>
     </row>
     <row r="182" spans="8:10" x14ac:dyDescent="0.45">
@@ -10145,10 +10181,10 @@
         <v>296</v>
       </c>
       <c r="I182" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="J182">
-        <v>1.213885486216326E-4</v>
+        <v>1.1611033929401374E-4</v>
       </c>
     </row>
     <row r="183" spans="8:10" x14ac:dyDescent="0.45">
@@ -10156,10 +10192,10 @@
         <v>296</v>
       </c>
       <c r="I183" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="J183">
-        <v>1.213885486216326E-4</v>
+        <v>1.1611033929401374E-4</v>
       </c>
     </row>
     <row r="184" spans="8:10" x14ac:dyDescent="0.45">
@@ -10167,10 +10203,10 @@
         <v>296</v>
       </c>
       <c r="I184" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="J184">
-        <v>1.2098160558030635E-4</v>
+        <v>1.1610133308926104E-4</v>
       </c>
     </row>
     <row r="185" spans="8:10" x14ac:dyDescent="0.45">
@@ -10178,10 +10214,10 @@
         <v>296</v>
       </c>
       <c r="I185" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="J185">
-        <v>1.1998772546014418E-4</v>
+        <v>1.1610133308926104E-4</v>
       </c>
     </row>
     <row r="186" spans="8:10" x14ac:dyDescent="0.45">
@@ -10189,10 +10225,10 @@
         <v>296</v>
       </c>
       <c r="I186" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="J186">
-        <v>1.1941080544078703E-4</v>
+        <v>1.1608872440260724E-4</v>
       </c>
     </row>
     <row r="187" spans="8:10" x14ac:dyDescent="0.45">
@@ -10200,10 +10236,10 @@
         <v>296</v>
       </c>
       <c r="I187" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="J187">
-        <v>1.1868018616505205E-4</v>
+        <v>1.1608872440260724E-4</v>
       </c>
     </row>
     <row r="188" spans="8:10" x14ac:dyDescent="0.45">
@@ -10211,10 +10247,10 @@
         <v>296</v>
       </c>
       <c r="I188" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="J188">
-        <v>1.1702956258281103E-4</v>
+        <v>1.1638142605707047E-4</v>
       </c>
     </row>
     <row r="189" spans="8:10" x14ac:dyDescent="0.45">
@@ -10222,10 +10258,10 @@
         <v>296</v>
       </c>
       <c r="I189" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="J189">
-        <v>1.1608326349517316E-4</v>
+        <v>1.1641474901465549E-4</v>
       </c>
     </row>
     <row r="190" spans="8:10" x14ac:dyDescent="0.45">
@@ -10233,10 +10269,10 @@
         <v>296</v>
       </c>
       <c r="I190" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="J190">
-        <v>1.1598246683416773E-4</v>
+        <v>1.1641474901465549E-4</v>
       </c>
     </row>
     <row r="191" spans="8:10" x14ac:dyDescent="0.45">
@@ -10244,10 +10280,10 @@
         <v>296</v>
       </c>
       <c r="I191" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="J191">
-        <v>1.1598246683416773E-4</v>
+        <v>1.1602448014203785E-4</v>
       </c>
     </row>
     <row r="192" spans="8:10" x14ac:dyDescent="0.45">
@@ -10255,10 +10291,10 @@
         <v>296</v>
       </c>
       <c r="I192" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="J192">
-        <v>1.1641601768973454E-4</v>
+        <v>1.1507132347237556E-4</v>
       </c>
     </row>
     <row r="193" spans="8:10" x14ac:dyDescent="0.45">
@@ -10266,10 +10302,10 @@
         <v>296</v>
       </c>
       <c r="I193" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="J193">
-        <v>1.182253490580928E-4</v>
+        <v>1.1451804229373379E-4</v>
       </c>
     </row>
     <row r="194" spans="8:10" x14ac:dyDescent="0.45">
@@ -10277,10 +10313,10 @@
         <v>296</v>
       </c>
       <c r="I194" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="J194">
-        <v>1.196753184176491E-4</v>
+        <v>1.1381735956397256E-4</v>
       </c>
     </row>
     <row r="195" spans="8:10" x14ac:dyDescent="0.45">
@@ -10288,10 +10324,10 @@
         <v>296</v>
       </c>
       <c r="I195" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="J195">
-        <v>1.2055024595650054E-4</v>
+        <v>1.122343689752704E-4</v>
       </c>
     </row>
     <row r="196" spans="8:10" x14ac:dyDescent="0.45">
@@ -10299,10 +10335,10 @@
         <v>296</v>
       </c>
       <c r="I196" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="J196">
-        <v>1.2093465061399949E-4</v>
+        <v>1.1172611882039221E-4</v>
       </c>
     </row>
     <row r="197" spans="8:10" x14ac:dyDescent="0.45">
@@ -10310,10 +10346,10 @@
         <v>296</v>
       </c>
       <c r="I197" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="J197">
-        <v>1.2105579442707122E-4</v>
+        <v>1.1132684374302186E-4</v>
       </c>
     </row>
     <row r="198" spans="8:10" x14ac:dyDescent="0.45">
@@ -10321,10 +10357,10 @@
         <v>296</v>
       </c>
       <c r="I198" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="J198">
-        <v>1.2098755320937189E-4</v>
+        <v>1.1123017714534272E-4</v>
       </c>
     </row>
     <row r="199" spans="8:10" x14ac:dyDescent="0.45">
@@ -10332,10 +10368,10 @@
         <v>296</v>
       </c>
       <c r="I199" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="J199">
-        <v>1.2091680772680286E-4</v>
+        <v>1.1123017714534272E-4</v>
       </c>
     </row>
     <row r="200" spans="8:10" x14ac:dyDescent="0.45">
@@ -10343,10 +10379,10 @@
         <v>296</v>
       </c>
       <c r="I200" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="J200">
-        <v>1.2082070656242813E-4</v>
+        <v>1.1164596359809305E-4</v>
       </c>
     </row>
     <row r="201" spans="8:10" x14ac:dyDescent="0.45">
@@ -10354,10 +10390,10 @@
         <v>296</v>
       </c>
       <c r="I201" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="J201">
-        <v>1.2077312552990384E-4</v>
+        <v>1.133811590471161E-4</v>
       </c>
     </row>
     <row r="202" spans="8:10" x14ac:dyDescent="0.45">
@@ -10365,10 +10401,10 @@
         <v>296</v>
       </c>
       <c r="I202" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="J202">
-        <v>1.2075966510622921E-4</v>
+        <v>1.1477171706093525E-4</v>
       </c>
     </row>
     <row r="203" spans="8:10" x14ac:dyDescent="0.45">
@@ -10376,10 +10412,10 @@
         <v>296</v>
       </c>
       <c r="I203" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="J203">
-        <v>1.208075591718622E-4</v>
+        <v>1.1561079513706318E-4</v>
       </c>
     </row>
     <row r="204" spans="8:10" x14ac:dyDescent="0.45">
@@ -10387,10 +10423,10 @@
         <v>296</v>
       </c>
       <c r="I204" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="J204">
-        <v>1.2133595905936891E-4</v>
+        <v>1.1597944911827429E-4</v>
       </c>
     </row>
     <row r="205" spans="8:10" x14ac:dyDescent="0.45">
@@ -10398,10 +10434,10 @@
         <v>296</v>
       </c>
       <c r="I205" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="J205">
-        <v>1.2138854862163262E-4</v>
+        <v>1.1609562915958431E-4</v>
       </c>
     </row>
     <row r="206" spans="8:10" x14ac:dyDescent="0.45">
@@ -10409,10 +10445,10 @@
         <v>296</v>
       </c>
       <c r="I206" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="J206">
-        <v>1.2147932822315923E-4</v>
+        <v>1.1603018407171459E-4</v>
       </c>
     </row>
     <row r="207" spans="8:10" x14ac:dyDescent="0.45">
@@ -10420,10 +10456,10 @@
         <v>296</v>
       </c>
       <c r="I207" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="J207">
-        <v>1.210304387452655E-4</v>
+        <v>1.1596233732924413E-4</v>
       </c>
     </row>
     <row r="208" spans="8:10" x14ac:dyDescent="0.45">
@@ -10431,10 +10467,10 @@
         <v>296</v>
       </c>
       <c r="I208" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="J208">
-        <v>1.1995955248036004E-4</v>
+        <v>1.1587017383394134E-4</v>
       </c>
     </row>
     <row r="209" spans="8:10" x14ac:dyDescent="0.45">
@@ -10442,10 +10478,10 @@
         <v>296</v>
       </c>
       <c r="I209" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="J209">
-        <v>1.1943522202326662E-4</v>
+        <v>1.1582454239652762E-4</v>
       </c>
     </row>
     <row r="210" spans="8:10" x14ac:dyDescent="0.45">
@@ -10453,10 +10489,10 @@
         <v>296</v>
       </c>
       <c r="I210" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="J210">
-        <v>1.1866140417852932E-4</v>
+        <v>1.1581163350304872E-4</v>
       </c>
     </row>
     <row r="211" spans="8:10" x14ac:dyDescent="0.45">
@@ -10464,10 +10500,98 @@
         <v>296</v>
       </c>
       <c r="I211" t="s">
+        <v>279</v>
+      </c>
+      <c r="J211">
+        <v>1.1585756514728754E-4</v>
+      </c>
+    </row>
+    <row r="212" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H212" t="s">
+        <v>296</v>
+      </c>
+      <c r="I212" t="s">
+        <v>280</v>
+      </c>
+      <c r="J212">
+        <v>1.163643142680403E-4</v>
+      </c>
+    </row>
+    <row r="213" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H213" t="s">
+        <v>296</v>
+      </c>
+      <c r="I213" t="s">
+        <v>281</v>
+      </c>
+      <c r="J213">
+        <v>1.1641474901465552E-4</v>
+      </c>
+    </row>
+    <row r="214" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H214" t="s">
+        <v>296</v>
+      </c>
+      <c r="I214" t="s">
+        <v>282</v>
+      </c>
+      <c r="J214">
+        <v>1.1650180899393174E-4</v>
+      </c>
+    </row>
+    <row r="215" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H215" t="s">
+        <v>296</v>
+      </c>
+      <c r="I215" t="s">
+        <v>283</v>
+      </c>
+      <c r="J215">
+        <v>1.1607131240675198E-4</v>
+      </c>
+    </row>
+    <row r="216" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H216" t="s">
+        <v>296</v>
+      </c>
+      <c r="I216" t="s">
+        <v>284</v>
+      </c>
+      <c r="J216">
+        <v>1.1504430485811741E-4</v>
+      </c>
+    </row>
+    <row r="217" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H217" t="s">
+        <v>296</v>
+      </c>
+      <c r="I217" t="s">
+        <v>285</v>
+      </c>
+      <c r="J217">
+        <v>1.1454145842609084E-4</v>
+      </c>
+    </row>
+    <row r="218" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H218" t="s">
+        <v>296</v>
+      </c>
+      <c r="I218" t="s">
         <v>286</v>
       </c>
-      <c r="J211">
-        <v>1.1704803153622508E-4</v>
+      <c r="J218">
+        <v>1.1379934715446716E-4</v>
+      </c>
+    </row>
+    <row r="219" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H219" t="s">
+        <v>296</v>
+      </c>
+      <c r="I219" t="s">
+        <v>287</v>
+      </c>
+      <c r="J219">
+        <v>1.1225208117795075E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>